<commit_message>
Completed raw freqs module E. Governance
</commit_message>
<xml_diff>
--- a/data/BPPS hh instrument pre-codebook.xlsx
+++ b/data/BPPS hh instrument pre-codebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Egnyte\Private\dkillian\AMELA\BPPS\workflowr\USAID Baseline Public Perception Survey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB04E76C-EBBD-4D27-AAE7-17046FB0A04D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB51D8F1-058E-4D44-B338-78CEADB7DD1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="917" firstSheet="11" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="917" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="varnames" sheetId="1" r:id="rId1"/>
@@ -2944,12 +2944,6 @@
     <t>Once a day or more</t>
   </si>
   <si>
-    <t>optimisim_code</t>
-  </si>
-  <si>
-    <t>optimisim_lab</t>
-  </si>
-  <si>
     <t>Very pessimistic</t>
   </si>
   <si>
@@ -3915,6 +3909,12 @@
   </si>
   <si>
     <t>Very bad job</t>
+  </si>
+  <si>
+    <t>optimism_code</t>
+  </si>
+  <si>
+    <t>optimism_lab</t>
   </si>
 </sst>
 </file>
@@ -4767,7 +4767,7 @@
         <v>45</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="G14" s="21"/>
     </row>
@@ -4788,7 +4788,7 @@
         <v>47</v>
       </c>
       <c r="F15" s="29" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="G15" s="21"/>
     </row>
@@ -4809,7 +4809,7 @@
         <v>49</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="G16" s="21"/>
     </row>
@@ -4851,7 +4851,7 @@
         <v>54</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="G18" s="21"/>
     </row>
@@ -4872,7 +4872,7 @@
         <v>56</v>
       </c>
       <c r="F19" s="29" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="G19" s="21"/>
     </row>
@@ -4893,7 +4893,7 @@
         <v>58</v>
       </c>
       <c r="F20" s="29" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="G20" s="21"/>
     </row>
@@ -4914,7 +4914,7 @@
         <v>60</v>
       </c>
       <c r="F21" s="29" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="G21" s="21"/>
     </row>
@@ -4956,7 +4956,7 @@
         <v>65</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="G23" s="21"/>
     </row>
@@ -4977,7 +4977,7 @@
         <v>67</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="G24" s="21"/>
     </row>
@@ -4998,7 +4998,7 @@
         <v>69</v>
       </c>
       <c r="F25" s="29" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="G25" s="21"/>
     </row>
@@ -5019,7 +5019,7 @@
         <v>71</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="G26" s="21"/>
     </row>
@@ -5040,7 +5040,7 @@
         <v>73</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="G27" s="21"/>
     </row>
@@ -5075,16 +5075,16 @@
         <v>74</v>
       </c>
       <c r="C29" s="24" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F29" s="28" t="s">
         <v>1130</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>1130</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>1131</v>
-      </c>
-      <c r="F29" s="28" t="s">
-        <v>1132</v>
       </c>
       <c r="G29" s="22"/>
     </row>
@@ -5096,16 +5096,16 @@
         <v>74</v>
       </c>
       <c r="C30" s="24" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>1131</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>1132</v>
+      </c>
+      <c r="F30" s="28" t="s">
         <v>1133</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>1133</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>1134</v>
-      </c>
-      <c r="F30" s="28" t="s">
-        <v>1135</v>
       </c>
       <c r="G30" s="22"/>
     </row>
@@ -5117,16 +5117,16 @@
         <v>74</v>
       </c>
       <c r="C31" s="24" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F31" s="28" t="s">
         <v>1136</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>1136</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>1137</v>
-      </c>
-      <c r="F31" s="28" t="s">
-        <v>1138</v>
       </c>
       <c r="G31" s="22"/>
     </row>
@@ -6006,7 +6006,7 @@
         <v>187</v>
       </c>
       <c r="F70" s="28" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="G70" s="22"/>
     </row>
@@ -6472,7 +6472,7 @@
         <v>253</v>
       </c>
       <c r="F92" s="28" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="G92" s="26"/>
     </row>
@@ -6493,7 +6493,7 @@
         <v>256</v>
       </c>
       <c r="F93" s="28" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="G93" s="26"/>
     </row>
@@ -6505,10 +6505,10 @@
         <v>161</v>
       </c>
       <c r="C94" s="24" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="D94" s="22" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="E94" s="22" t="s">
         <v>257</v>
@@ -6526,10 +6526,10 @@
         <v>161</v>
       </c>
       <c r="C95" s="24" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="D95" s="22" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="E95" s="22" t="s">
         <v>259</v>
@@ -6547,10 +6547,10 @@
         <v>161</v>
       </c>
       <c r="C96" s="24" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="D96" s="22" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="E96" s="22" t="s">
         <v>261</v>
@@ -6594,7 +6594,7 @@
         <v>266</v>
       </c>
       <c r="D98" s="22" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="E98" s="22" t="s">
         <v>267</v>
@@ -6617,7 +6617,7 @@
         <v>297</v>
       </c>
       <c r="D99" s="22" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="E99" s="22" t="s">
         <v>298</v>
@@ -6640,7 +6640,7 @@
         <v>270</v>
       </c>
       <c r="D100" s="22" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="E100" s="22" t="s">
         <v>271</v>
@@ -6663,7 +6663,7 @@
         <v>299</v>
       </c>
       <c r="D101" s="22" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="E101" s="22" t="s">
         <v>300</v>
@@ -6686,7 +6686,7 @@
         <v>273</v>
       </c>
       <c r="D102" s="22" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="E102" s="22" t="s">
         <v>274</v>
@@ -6709,7 +6709,7 @@
         <v>301</v>
       </c>
       <c r="D103" s="22" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="E103" s="22" t="s">
         <v>302</v>
@@ -6732,7 +6732,7 @@
         <v>276</v>
       </c>
       <c r="D104" s="22" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="E104" s="22" t="s">
         <v>277</v>
@@ -6755,7 +6755,7 @@
         <v>303</v>
       </c>
       <c r="D105" s="22" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="E105" s="22" t="s">
         <v>304</v>
@@ -6778,7 +6778,7 @@
         <v>279</v>
       </c>
       <c r="D106" s="22" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="E106" s="22" t="s">
         <v>280</v>
@@ -6801,7 +6801,7 @@
         <v>305</v>
       </c>
       <c r="D107" s="22" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="E107" s="22" t="s">
         <v>306</v>
@@ -6824,7 +6824,7 @@
         <v>282</v>
       </c>
       <c r="D108" s="22" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="E108" s="22" t="s">
         <v>283</v>
@@ -6847,7 +6847,7 @@
         <v>307</v>
       </c>
       <c r="D109" s="22" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="E109" s="22" t="s">
         <v>308</v>
@@ -6870,7 +6870,7 @@
         <v>285</v>
       </c>
       <c r="D110" s="22" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="E110" s="22" t="s">
         <v>286</v>
@@ -6893,7 +6893,7 @@
         <v>309</v>
       </c>
       <c r="D111" s="22" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="E111" s="22" t="s">
         <v>310</v>
@@ -6916,7 +6916,7 @@
         <v>288</v>
       </c>
       <c r="D112" s="22" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="E112" s="22" t="s">
         <v>289</v>
@@ -6939,7 +6939,7 @@
         <v>311</v>
       </c>
       <c r="D113" s="22" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E113" s="22" t="s">
         <v>312</v>
@@ -6962,7 +6962,7 @@
         <v>291</v>
       </c>
       <c r="D114" s="22" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="E114" s="22" t="s">
         <v>292</v>
@@ -6985,7 +6985,7 @@
         <v>313</v>
       </c>
       <c r="D115" s="22" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="E115" s="22" t="s">
         <v>314</v>
@@ -7008,7 +7008,7 @@
         <v>294</v>
       </c>
       <c r="D116" s="22" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="E116" s="22" t="s">
         <v>295</v>
@@ -7031,7 +7031,7 @@
         <v>315</v>
       </c>
       <c r="D117" s="22" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="E117" s="22" t="s">
         <v>316</v>
@@ -7140,7 +7140,7 @@
         <v>330</v>
       </c>
       <c r="D122" s="22" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="E122" s="22" t="s">
         <v>331</v>
@@ -7163,7 +7163,7 @@
         <v>363</v>
       </c>
       <c r="D123" s="22" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="E123" s="22" t="s">
         <v>364</v>
@@ -7186,7 +7186,7 @@
         <v>385</v>
       </c>
       <c r="D124" s="22" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="E124" s="22" t="s">
         <v>386</v>
@@ -7209,7 +7209,7 @@
         <v>333</v>
       </c>
       <c r="D125" s="22" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="E125" s="22" t="s">
         <v>334</v>
@@ -7232,7 +7232,7 @@
         <v>365</v>
       </c>
       <c r="D126" s="22" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="E126" s="22" t="s">
         <v>366</v>
@@ -7255,7 +7255,7 @@
         <v>388</v>
       </c>
       <c r="D127" s="22" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="E127" s="22" t="s">
         <v>389</v>
@@ -7278,7 +7278,7 @@
         <v>336</v>
       </c>
       <c r="D128" s="22" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="E128" s="22" t="s">
         <v>337</v>
@@ -7301,7 +7301,7 @@
         <v>367</v>
       </c>
       <c r="D129" s="22" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="E129" s="22" t="s">
         <v>368</v>
@@ -7324,7 +7324,7 @@
         <v>390</v>
       </c>
       <c r="D130" s="22" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="E130" s="22" t="s">
         <v>391</v>
@@ -7347,7 +7347,7 @@
         <v>339</v>
       </c>
       <c r="D131" s="22" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="E131" s="22" t="s">
         <v>340</v>
@@ -7370,7 +7370,7 @@
         <v>369</v>
       </c>
       <c r="D132" s="22" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="E132" s="22" t="s">
         <v>370</v>
@@ -7393,7 +7393,7 @@
         <v>392</v>
       </c>
       <c r="D133" s="22" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="E133" s="22" t="s">
         <v>393</v>
@@ -7416,7 +7416,7 @@
         <v>342</v>
       </c>
       <c r="D134" s="22" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="E134" s="22" t="s">
         <v>343</v>
@@ -7439,7 +7439,7 @@
         <v>371</v>
       </c>
       <c r="D135" s="22" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="E135" s="22" t="s">
         <v>372</v>
@@ -7462,7 +7462,7 @@
         <v>394</v>
       </c>
       <c r="D136" s="22" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="E136" s="22" t="s">
         <v>395</v>
@@ -7485,7 +7485,7 @@
         <v>345</v>
       </c>
       <c r="D137" s="22" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="E137" s="22" t="s">
         <v>346</v>
@@ -7508,7 +7508,7 @@
         <v>373</v>
       </c>
       <c r="D138" s="22" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="E138" s="22" t="s">
         <v>374</v>
@@ -7531,7 +7531,7 @@
         <v>396</v>
       </c>
       <c r="D139" s="22" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="E139" s="22" t="s">
         <v>397</v>
@@ -7554,7 +7554,7 @@
         <v>348</v>
       </c>
       <c r="D140" s="22" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="E140" s="22" t="s">
         <v>349</v>
@@ -7577,7 +7577,7 @@
         <v>375</v>
       </c>
       <c r="D141" s="22" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="E141" s="22" t="s">
         <v>376</v>
@@ -7600,7 +7600,7 @@
         <v>398</v>
       </c>
       <c r="D142" s="22" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="E142" s="22" t="s">
         <v>399</v>
@@ -7623,7 +7623,7 @@
         <v>351</v>
       </c>
       <c r="D143" s="22" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="E143" s="22" t="s">
         <v>352</v>
@@ -7646,7 +7646,7 @@
         <v>377</v>
       </c>
       <c r="D144" s="22" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="E144" s="22" t="s">
         <v>378</v>
@@ -7669,7 +7669,7 @@
         <v>400</v>
       </c>
       <c r="D145" s="22" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E145" s="22" t="s">
         <v>401</v>
@@ -7692,7 +7692,7 @@
         <v>354</v>
       </c>
       <c r="D146" s="22" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="E146" s="22" t="s">
         <v>355</v>
@@ -7715,7 +7715,7 @@
         <v>379</v>
       </c>
       <c r="D147" s="22" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E147" s="22" t="s">
         <v>380</v>
@@ -7738,7 +7738,7 @@
         <v>402</v>
       </c>
       <c r="D148" s="22" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="E148" s="22" t="s">
         <v>403</v>
@@ -7761,7 +7761,7 @@
         <v>357</v>
       </c>
       <c r="D149" s="22" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="E149" s="22" t="s">
         <v>358</v>
@@ -7784,7 +7784,7 @@
         <v>381</v>
       </c>
       <c r="D150" s="22" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="E150" s="22" t="s">
         <v>382</v>
@@ -7807,7 +7807,7 @@
         <v>404</v>
       </c>
       <c r="D151" s="22" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="E151" s="22" t="s">
         <v>405</v>
@@ -7830,7 +7830,7 @@
         <v>360</v>
       </c>
       <c r="D152" s="22" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="E152" s="22" t="s">
         <v>361</v>
@@ -7853,7 +7853,7 @@
         <v>383</v>
       </c>
       <c r="D153" s="22" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="E153" s="22" t="s">
         <v>384</v>
@@ -7876,7 +7876,7 @@
         <v>406</v>
       </c>
       <c r="D154" s="22" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="E154" s="22" t="s">
         <v>407</v>
@@ -7896,14 +7896,14 @@
         <v>329</v>
       </c>
       <c r="C155" s="22" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="D155" s="22" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="E155" s="22"/>
       <c r="F155" s="27" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="G155" s="25"/>
     </row>
@@ -7915,14 +7915,14 @@
         <v>329</v>
       </c>
       <c r="C156" s="22" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="D156" s="22" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="E156" s="22"/>
       <c r="F156" s="27" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="G156" s="25"/>
     </row>
@@ -7934,14 +7934,14 @@
         <v>329</v>
       </c>
       <c r="C157" s="22" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="D157" s="22" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="E157" s="22"/>
       <c r="F157" s="27" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="G157" s="25"/>
     </row>
@@ -7953,14 +7953,14 @@
         <v>329</v>
       </c>
       <c r="C158" s="22" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="D158" s="22" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="E158" s="22"/>
       <c r="F158" s="27" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="G158" s="25"/>
     </row>
@@ -7972,14 +7972,14 @@
         <v>329</v>
       </c>
       <c r="C159" s="22" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="D159" s="22" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="E159" s="22"/>
       <c r="F159" s="27" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="G159" s="25"/>
     </row>
@@ -7991,14 +7991,14 @@
         <v>329</v>
       </c>
       <c r="C160" s="22" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="D160" s="22" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="E160" s="22"/>
       <c r="F160" s="27" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="G160" s="25"/>
     </row>
@@ -8013,7 +8013,7 @@
         <v>408</v>
       </c>
       <c r="D161" s="22" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="E161" s="22" t="s">
         <v>409</v>
@@ -8036,7 +8036,7 @@
         <v>429</v>
       </c>
       <c r="D162" s="22" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="E162" s="22" t="s">
         <v>430</v>
@@ -8059,7 +8059,7 @@
         <v>411</v>
       </c>
       <c r="D163" s="22" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="E163" s="22" t="s">
         <v>412</v>
@@ -8082,7 +8082,7 @@
         <v>431</v>
       </c>
       <c r="D164" s="22" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="E164" s="22" t="s">
         <v>432</v>
@@ -8105,7 +8105,7 @@
         <v>414</v>
       </c>
       <c r="D165" s="22" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="E165" s="22" t="s">
         <v>415</v>
@@ -8128,7 +8128,7 @@
         <v>433</v>
       </c>
       <c r="D166" s="22" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="E166" s="22" t="s">
         <v>434</v>
@@ -8151,7 +8151,7 @@
         <v>417</v>
       </c>
       <c r="D167" s="22" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="E167" s="22" t="s">
         <v>418</v>
@@ -8174,7 +8174,7 @@
         <v>435</v>
       </c>
       <c r="D168" s="22" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="E168" s="22" t="s">
         <v>436</v>
@@ -8197,7 +8197,7 @@
         <v>420</v>
       </c>
       <c r="D169" s="22" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="E169" s="22" t="s">
         <v>421</v>
@@ -8220,7 +8220,7 @@
         <v>437</v>
       </c>
       <c r="D170" s="22" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="E170" s="22" t="s">
         <v>438</v>
@@ -8243,7 +8243,7 @@
         <v>423</v>
       </c>
       <c r="D171" s="22" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="E171" s="22" t="s">
         <v>424</v>
@@ -8266,7 +8266,7 @@
         <v>439</v>
       </c>
       <c r="D172" s="22" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="E172" s="22" t="s">
         <v>440</v>
@@ -8289,7 +8289,7 @@
         <v>426</v>
       </c>
       <c r="D173" s="22" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="E173" s="22" t="s">
         <v>427</v>
@@ -8312,7 +8312,7 @@
         <v>441</v>
       </c>
       <c r="D174" s="22" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="E174" s="22" t="s">
         <v>442</v>
@@ -8387,7 +8387,7 @@
         <v>451</v>
       </c>
       <c r="F177" s="30" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="G177" s="25" t="s">
         <v>446</v>
@@ -8502,7 +8502,7 @@
         <v>464</v>
       </c>
       <c r="F182" s="27" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="G182" s="22"/>
     </row>
@@ -8523,7 +8523,7 @@
         <v>466</v>
       </c>
       <c r="F183" s="27" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="G183" s="22"/>
     </row>
@@ -8544,7 +8544,7 @@
         <v>468</v>
       </c>
       <c r="F184" s="27" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="G184" s="22"/>
     </row>
@@ -8565,7 +8565,7 @@
         <v>470</v>
       </c>
       <c r="F185" s="27" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="G185" s="22"/>
     </row>
@@ -8808,13 +8808,13 @@
         <v>329</v>
       </c>
       <c r="C197" s="22" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="D197" s="22" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="E197" s="22" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="F197" s="28" t="s">
         <v>529</v>
@@ -8829,10 +8829,10 @@
         <v>329</v>
       </c>
       <c r="C198" s="22" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="D198" s="22" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="E198" s="22" t="s">
         <v>498</v>
@@ -8850,10 +8850,10 @@
         <v>329</v>
       </c>
       <c r="C199" s="22" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="D199" s="22" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="E199" s="22" t="s">
         <v>499</v>
@@ -9086,7 +9086,7 @@
         <v>530</v>
       </c>
       <c r="D210" s="22" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="E210" s="22" t="s">
         <v>531</v>
@@ -9107,7 +9107,7 @@
         <v>532</v>
       </c>
       <c r="D211" s="22" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="E211" s="22" t="s">
         <v>533</v>
@@ -9128,7 +9128,7 @@
         <v>534</v>
       </c>
       <c r="D212" s="22" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E212" s="22" t="s">
         <v>535</v>
@@ -9551,7 +9551,7 @@
         <v>596</v>
       </c>
       <c r="F231" s="27" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="G231" s="26"/>
     </row>
@@ -9564,11 +9564,11 @@
       </c>
       <c r="C232" s="24"/>
       <c r="D232" s="22" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="E232" s="22"/>
       <c r="F232" s="31" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="G232" s="26"/>
     </row>
@@ -9581,7 +9581,7 @@
       </c>
       <c r="C233" s="24"/>
       <c r="D233" s="22" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="E233" s="22"/>
       <c r="F233" s="27" t="s">
@@ -9598,7 +9598,7 @@
       </c>
       <c r="C234" s="24"/>
       <c r="D234" s="22" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="E234" s="22"/>
       <c r="F234" s="28" t="s">
@@ -9615,7 +9615,7 @@
       </c>
       <c r="C235" s="24"/>
       <c r="D235" s="22" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="E235" s="22"/>
       <c r="F235" s="27" t="s">
@@ -9640,7 +9640,7 @@
         <v>599</v>
       </c>
       <c r="F236" s="28" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="G236" s="25" t="s">
         <v>600</v>
@@ -9663,7 +9663,7 @@
         <v>602</v>
       </c>
       <c r="F237" s="28" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="G237" s="25" t="s">
         <v>600</v>
@@ -9965,7 +9965,7 @@
         <v>646</v>
       </c>
       <c r="F251" s="27" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="G251" s="26"/>
     </row>
@@ -9983,7 +9983,7 @@
         <v>647</v>
       </c>
       <c r="F252" s="31" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="G252" s="26"/>
     </row>
@@ -9995,10 +9995,10 @@
         <v>597</v>
       </c>
       <c r="C253" s="22" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="D253" s="22" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="E253" s="22" t="s">
         <v>648</v>
@@ -10016,10 +10016,10 @@
         <v>597</v>
       </c>
       <c r="C254" s="22" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="D254" s="22" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="E254" s="22" t="s">
         <v>650</v>
@@ -10037,10 +10037,10 @@
         <v>597</v>
       </c>
       <c r="C255" s="22" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="D255" s="22" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="E255" s="22" t="s">
         <v>652</v>
@@ -10081,10 +10081,10 @@
         <v>597</v>
       </c>
       <c r="C257" s="24" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="D257" s="22" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="E257" s="22" t="s">
         <v>656</v>
@@ -10102,10 +10102,10 @@
         <v>597</v>
       </c>
       <c r="C258" s="24" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="D258" s="22" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="E258" s="22" t="s">
         <v>657</v>
@@ -10123,10 +10123,10 @@
         <v>597</v>
       </c>
       <c r="C259" s="24" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="D259" s="22" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="E259" s="22" t="s">
         <v>658</v>
@@ -10144,10 +10144,10 @@
         <v>597</v>
       </c>
       <c r="C260" s="24" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="D260" s="22" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="E260" s="22" t="s">
         <v>659</v>
@@ -10165,10 +10165,10 @@
         <v>597</v>
       </c>
       <c r="C261" s="24" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="D261" s="22" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="E261" s="22" t="s">
         <v>660</v>
@@ -10186,10 +10186,10 @@
         <v>597</v>
       </c>
       <c r="C262" s="24" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="D262" s="22" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="E262" s="22" t="s">
         <v>661</v>
@@ -10207,10 +10207,10 @@
         <v>597</v>
       </c>
       <c r="C263" s="24" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="D263" s="22" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="E263" s="22" t="s">
         <v>662</v>
@@ -10249,10 +10249,10 @@
         <v>597</v>
       </c>
       <c r="C265" s="24" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="D265" s="22" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="E265" s="22" t="s">
         <v>665</v>
@@ -10273,7 +10273,7 @@
         <v>642</v>
       </c>
       <c r="D266" s="22" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="E266" s="22" t="s">
         <v>666</v>
@@ -10294,13 +10294,13 @@
         <v>645</v>
       </c>
       <c r="D267" s="22" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="E267" s="22" t="s">
         <v>667</v>
       </c>
       <c r="F267" s="27" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="G267" s="26"/>
     </row>
@@ -10315,10 +10315,10 @@
         <v>647</v>
       </c>
       <c r="D268" s="22" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="F268" s="31" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="G268" s="26"/>
     </row>
@@ -10333,7 +10333,7 @@
         <v>649</v>
       </c>
       <c r="D269" s="22" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="E269" s="22" t="s">
         <v>668</v>
@@ -10354,7 +10354,7 @@
         <v>651</v>
       </c>
       <c r="D270" s="22" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="E270" s="22" t="s">
         <v>669</v>
@@ -10373,7 +10373,7 @@
       </c>
       <c r="C271" s="24"/>
       <c r="D271" s="22" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="E271" s="22" t="s">
         <v>670</v>
@@ -10625,7 +10625,7 @@
         <v>703</v>
       </c>
       <c r="D283" s="22" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="E283" s="22" t="s">
         <v>704</v>
@@ -10646,7 +10646,7 @@
         <v>705</v>
       </c>
       <c r="D284" s="22" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="E284" s="22" t="s">
         <v>706</v>
@@ -11553,7 +11553,7 @@
         <v>837</v>
       </c>
       <c r="F326" s="28" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="G326" s="22" t="s">
         <v>837</v>
@@ -11576,7 +11576,7 @@
         <v>839</v>
       </c>
       <c r="F327" s="28" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="G327" s="22"/>
     </row>
@@ -11589,11 +11589,11 @@
       </c>
       <c r="C328" s="24"/>
       <c r="D328" s="22" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="E328" s="22"/>
       <c r="F328" s="28" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="G328" s="33"/>
     </row>
@@ -12233,10 +12233,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="B1" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -12244,7 +12244,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -12252,7 +12252,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -12260,7 +12260,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -12268,7 +12268,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -12276,7 +12276,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -12284,7 +12284,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -12292,7 +12292,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -12300,7 +12300,7 @@
         <v>97</v>
       </c>
       <c r="B9" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -12889,16 +12889,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>956</v>
+        <v>1274</v>
       </c>
       <c r="B1" t="s">
-        <v>957</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -12906,7 +12908,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -12914,7 +12916,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -12922,7 +12924,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -12930,7 +12932,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -12938,7 +12940,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -13027,7 +13029,7 @@
         <v>567</v>
       </c>
       <c r="B1" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -13035,7 +13037,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -13043,7 +13045,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -13051,7 +13053,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -13059,7 +13061,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -13067,7 +13069,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -13114,7 +13116,7 @@
         <v>559</v>
       </c>
       <c r="B1" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -13122,7 +13124,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -13130,7 +13132,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -13146,7 +13148,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -13154,7 +13156,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -13205,10 +13207,10 @@
         <v>387</v>
       </c>
       <c r="B1" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="C1" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -13216,10 +13218,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -13227,10 +13229,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -13238,10 +13240,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -13249,10 +13251,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -13260,10 +13262,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -13271,7 +13273,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>129</v>
@@ -13282,10 +13284,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -13293,10 +13295,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -13304,10 +13306,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -13315,10 +13317,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -13326,10 +13328,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -13337,10 +13339,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -13388,7 +13390,7 @@
         <v>446</v>
       </c>
       <c r="B1" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -13396,7 +13398,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -13404,7 +13406,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -13412,7 +13414,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -13420,7 +13422,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -13459,7 +13461,7 @@
         <v>712</v>
       </c>
       <c r="B1" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -13467,7 +13469,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -13475,7 +13477,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -13483,7 +13485,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -13491,7 +13493,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -13499,7 +13501,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -13539,10 +13541,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="B1" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -13670,10 +13672,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="B1" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -13784,7 +13786,7 @@
         <v>541</v>
       </c>
       <c r="B1" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -13792,7 +13794,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -13800,7 +13802,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -13828,7 +13830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B45B07-324D-414C-9B01-F4192D1CC666}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -13839,10 +13841,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="B1" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -13850,7 +13852,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -13858,7 +13860,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -13866,7 +13868,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -13874,7 +13876,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -13917,7 +13919,7 @@
         <v>575</v>
       </c>
       <c r="B1" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -13925,7 +13927,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -13933,7 +13935,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -13941,7 +13943,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -14020,10 +14022,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="B1" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -14104,7 +14106,7 @@
         <v>600</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -14136,7 +14138,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -14202,10 +14204,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="B1" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -14324,7 +14326,7 @@
         <v>722</v>
       </c>
       <c r="B1" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -14332,7 +14334,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -14340,7 +14342,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -14348,7 +14350,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -14356,7 +14358,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -14395,7 +14397,7 @@
         <v>716</v>
       </c>
       <c r="B1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -14403,7 +14405,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -14411,7 +14413,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -14419,7 +14421,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -14427,7 +14429,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -14435,7 +14437,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -14476,7 +14478,7 @@
         <v>612</v>
       </c>
       <c r="B1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -14492,7 +14494,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -14500,7 +14502,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -14508,7 +14510,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -14547,7 +14549,7 @@
         <v>734</v>
       </c>
       <c r="B1" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -14555,7 +14557,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -14563,7 +14565,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -14571,7 +14573,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -14579,7 +14581,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -14587,7 +14589,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -14595,7 +14597,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -14603,7 +14605,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -14611,7 +14613,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -14619,7 +14621,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -14627,7 +14629,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -14635,7 +14637,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -14643,7 +14645,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -14651,7 +14653,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -14659,7 +14661,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -14667,7 +14669,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -14675,7 +14677,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -14721,10 +14723,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -14870,7 +14872,7 @@
         <v>837</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -14878,7 +14880,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -14886,7 +14888,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
     </row>
   </sheetData>
@@ -14909,10 +14911,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -14920,7 +14922,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -14928,7 +14930,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
     </row>
   </sheetData>
@@ -14951,10 +14953,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="B1" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -14962,7 +14964,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -14970,7 +14972,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -14978,7 +14980,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -14986,7 +14988,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -14994,7 +14996,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -15002,7 +15004,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -15010,7 +15012,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -15018,7 +15020,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -15026,7 +15028,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -15034,7 +15036,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -15042,7 +15044,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -15050,7 +15052,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -15058,7 +15060,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -15066,7 +15068,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
     </row>
   </sheetData>
@@ -15087,7 +15089,7 @@
         <v>850</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -15095,7 +15097,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -15103,7 +15105,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -15111,7 +15113,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -15119,7 +15121,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -15127,7 +15129,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -15170,7 +15172,7 @@
         <v>869</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -15178,7 +15180,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -15186,7 +15188,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -15194,7 +15196,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -15202,7 +15204,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -15233,7 +15235,7 @@
         <v>872</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -15241,7 +15243,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -15249,7 +15251,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -15257,7 +15259,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -15265,7 +15267,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
     </row>
   </sheetData>
@@ -15292,7 +15294,7 @@
         <v>878</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -15300,7 +15302,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -15308,7 +15310,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -15316,7 +15318,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -15324,7 +15326,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -15332,7 +15334,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
     </row>
   </sheetData>
@@ -15358,7 +15360,7 @@
         <v>853</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -15366,7 +15368,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -15374,7 +15376,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -15382,7 +15384,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -15390,7 +15392,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -15398,7 +15400,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -15406,7 +15408,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -15414,7 +15416,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -15422,7 +15424,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -15430,7 +15432,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -15438,7 +15440,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -15446,7 +15448,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -15454,7 +15456,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -15462,7 +15464,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -15470,7 +15472,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -15478,7 +15480,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -15784,7 +15786,7 @@
         <v>913</v>
       </c>
       <c r="B1" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -15833,21 +15835,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100672393E543181D44A14B926842EAEF86" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4f7d009885df2d94de87ac57354edbe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1bc6f98d-9bb8-4f09-93f0-a2681e7d463b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cce7b25449546cf6e85fdbff4f964c6f" ns2:_="">
     <xsd:import namespace="1bc6f98d-9bb8-4f09-93f0-a2681e7d463b"/>
@@ -16025,10 +16012,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3D330BE-5E44-498F-AC6A-46F929BFA84E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1173640-FCC7-4E72-8021-60B50F508150}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1bc6f98d-9bb8-4f09-93f0-a2681e7d463b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -16050,19 +16062,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1173640-FCC7-4E72-8021-60B50F508150}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3D330BE-5E44-498F-AC6A-46F929BFA84E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1bc6f98d-9bb8-4f09-93f0-a2681e7d463b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>